<commit_message>
reclassified start and stop
Former-commit-id: 419fa49d973bffb745e8b1c602327eed033d35ea
</commit_message>
<xml_diff>
--- a/Classifications/ClassifiedPhrases_Vids456.xlsx
+++ b/Classifications/ClassifiedPhrases_Vids456.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgandeneve/Documents/_HawCHI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgandeneve/Documents/GitHub/aerobictextreview/Classifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44E0ECCE-229C-B74B-A7A4-42294386FC2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836FF16A-A8FC-6640-B28D-9F1971FC8502}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10220" yWindow="500" windowWidth="23380" windowHeight="17360" activeTab="2" xr2:uid="{F0159C2B-3A58-4A49-BDFE-0BEE50612833}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23380" windowHeight="19420" activeTab="1" xr2:uid="{F0159C2B-3A58-4A49-BDFE-0BEE50612833}"/>
   </bookViews>
   <sheets>
     <sheet name="body-based" sheetId="1" r:id="rId1"/>
     <sheet name="time-based" sheetId="2" r:id="rId2"/>
     <sheet name="otherwise" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1929,11 +1929,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE17EC2-4C61-2441-887C-8BF1000E45B4}">
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96:B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3809,6 +3809,22 @@
         <v>273</v>
       </c>
     </row>
+    <row r="95" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>4</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>4</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3816,11 +3832,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0A333D-19C4-7B4B-88FB-0730E1537642}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31:H31"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3860,12 +3876,6 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="C2">
         <v>5</v>
       </c>
@@ -4087,12 +4097,12 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>249</v>
+        <v>312</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -4127,10 +4137,10 @@
     </row>
     <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -4138,6 +4148,12 @@
       <c r="D9" s="1" t="s">
         <v>293</v>
       </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>301</v>
+      </c>
       <c r="G9">
         <v>4</v>
       </c>
@@ -4159,10 +4175,10 @@
     </row>
     <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -4189,12 +4205,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>251</v>
+        <v>312</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -4226,7 +4242,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="C12">
         <v>6</v>
@@ -4252,7 +4268,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -4273,12 +4289,12 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>313</v>
+        <v>342</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -4304,7 +4320,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -4330,7 +4346,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -4351,13 +4367,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>312</v>
-      </c>
+    <row r="17" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C17">
         <v>6</v>
       </c>
@@ -4377,13 +4387,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>332</v>
-      </c>
+    <row r="18" spans="3:12" ht="34" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>6</v>
       </c>
@@ -4403,13 +4407,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>332</v>
-      </c>
+    <row r="19" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>6</v>
       </c>
@@ -4429,13 +4427,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>342</v>
-      </c>
+    <row r="20" spans="3:12" ht="68" x14ac:dyDescent="0.2">
       <c r="C20">
         <v>6</v>
       </c>
@@ -4455,13 +4447,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>322</v>
-      </c>
+    <row r="21" spans="3:12" ht="51" x14ac:dyDescent="0.2">
       <c r="C21">
         <v>6</v>
       </c>
@@ -4481,13 +4467,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>347</v>
-      </c>
+    <row r="22" spans="3:12" ht="51" x14ac:dyDescent="0.2">
       <c r="C22">
         <v>6</v>
       </c>
@@ -4507,13 +4487,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>362</v>
-      </c>
+    <row r="23" spans="3:12" ht="34" x14ac:dyDescent="0.2">
       <c r="C23">
         <v>6</v>
       </c>
@@ -4533,7 +4507,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="G24">
         <v>6</v>
       </c>
@@ -4547,7 +4521,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:12" ht="34" x14ac:dyDescent="0.2">
       <c r="G25">
         <v>6</v>
       </c>
@@ -4561,7 +4535,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:12" ht="51" x14ac:dyDescent="0.2">
       <c r="G26">
         <v>6</v>
       </c>
@@ -4575,7 +4549,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:12" ht="34" x14ac:dyDescent="0.2">
       <c r="G27">
         <v>6</v>
       </c>
@@ -4589,7 +4563,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="G28">
         <v>5</v>
       </c>
@@ -4603,7 +4577,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="G29">
         <v>5</v>
       </c>
@@ -4617,7 +4591,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="G30">
         <v>6</v>
       </c>
@@ -4631,7 +4605,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:12" ht="51" x14ac:dyDescent="0.2">
       <c r="G31">
         <v>6</v>
       </c>
@@ -4645,7 +4619,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:12" ht="51" x14ac:dyDescent="0.2">
       <c r="K32">
         <v>4</v>
       </c>
@@ -4715,6 +4689,46 @@
       </c>
       <c r="L40" s="1" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="11:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <v>6</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="42" spans="11:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <v>5</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="11:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <v>6</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="44" spans="11:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <v>4</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="45" spans="11:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <v>6</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -4726,8 +4740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE64671-A259-764C-A3BB-346630DCCC4A}">
   <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C97" sqref="C97:D98"/>
     </sheetView>
   </sheetViews>

</xml_diff>